<commit_message>
add english image view
</commit_message>
<xml_diff>
--- a/imageNumber.xlsx
+++ b/imageNumber.xlsx
@@ -299,7 +299,7 @@
     <t>35</t>
   </si>
   <si>
-    <t>img/35-1.png,img/35-2.png</t>
+    <t>img/35.png</t>
   </si>
   <si>
     <t>36</t>
@@ -359,7 +359,7 @@
     <t>45</t>
   </si>
   <si>
-    <t>img/45-1.png,img/45-2.png</t>
+    <t>img/45-1.png,img/45.png</t>
   </si>
   <si>
     <t>46</t>

</xml_diff>